<commit_message>
normalizer pontos em numeros
</commit_message>
<xml_diff>
--- a/planilhas/outputs/Categorizados.xlsx
+++ b/planilhas/outputs/Categorizados.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="1021">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="1030">
   <si>
     <t xml:space="preserve">FITAS E  ADESIVOS</t>
   </si>
@@ -3115,6 +3115,9 @@
     <t xml:space="preserve">CARINHO PEDREIRO</t>
   </si>
   <si>
+    <t xml:space="preserve">BUCHA REDUCAO ROSCA 3/4X1/2 50 KRONA</t>
+  </si>
+  <si>
     <t xml:space="preserve">SUPORTE PRIMETECH</t>
   </si>
   <si>
@@ -3127,6 +3130,9 @@
     <t xml:space="preserve">SERRA A R BOSCH BIMET 18D</t>
   </si>
   <si>
+    <t xml:space="preserve">BUCHA REDUCAO LL LONGA PLASTILIT 50 X 25</t>
+  </si>
+  <si>
     <t xml:space="preserve">MAQUINA LAVAR</t>
   </si>
   <si>
@@ -3139,6 +3145,9 @@
     <t xml:space="preserve">CARRINHO SERV GERAL ESFERA 150K P MACICO</t>
   </si>
   <si>
+    <t xml:space="preserve">BUCHA REDUCAO RR PLASTILIT A 3/4 X 1/2 BRANCO</t>
+  </si>
+  <si>
     <t xml:space="preserve">OVERTIME CHUVEIRINHO P/ TORNEIRA</t>
   </si>
   <si>
@@ -3151,6 +3160,9 @@
     <t xml:space="preserve">CHAVE DE RODA CRUZ IMA</t>
   </si>
   <si>
+    <t xml:space="preserve">BUCHA REDUCAO LL CURTA CORRER PLASTICO B 1 X 3/4</t>
+  </si>
+  <si>
     <t xml:space="preserve">PRIME TECH SUPORTE FORNO BRANCO</t>
   </si>
   <si>
@@ -3160,16 +3172,31 @@
     <t xml:space="preserve">ESTRELA VALVULA RETENÇÃO LL VERT/HOR PVC 32MM</t>
   </si>
   <si>
+    <t xml:space="preserve">BUCHA REDUCAO RR CORRER PLASTIK 3/4X1/2 BRANCO</t>
+  </si>
+  <si>
     <t xml:space="preserve">MANGUEIRA MAQUINA DE LAVAR ENTRADA 120MT IBIRA</t>
   </si>
   <si>
     <t xml:space="preserve">FILTRO LINHA MEGATRON 5TOM BIVOLT PRETO</t>
   </si>
   <si>
+    <t xml:space="preserve">BUCHA AUMENTO GARDEN 1/2 X3 /4 ZAMAC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BUCHA REDUCAO LL CURTA FORTL A 3/4X1/2 MARRO</t>
+  </si>
+  <si>
     <t xml:space="preserve">MANGUEIRA MAQUINA DE LAVAR ENTRADA 140MT IBIRA</t>
   </si>
   <si>
     <t xml:space="preserve">FILTRO LINHA MEGATRON 4TOM BIVOLT PRETO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BUCHA REDUCAO GARDEN 3/4 X 1/2 ZAMAC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BUCHA REDUCAO LL LONGA FORT C 1 1/2 X3/4</t>
   </si>
   <si>
     <t xml:space="preserve">MANGUEIRA ENTRADA NOVA 14M</t>
@@ -3304,7 +3331,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3322,10 +3349,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3462,8 +3485,8 @@
   </sheetPr>
   <dimension ref="A1:AF91"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H67" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H84" activeCellId="0" sqref="H84"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Y59" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Z79" activeCellId="0" sqref="Z78:Z81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5366,7 +5389,7 @@
       <c r="F27" s="1" t="s">
         <v>596</v>
       </c>
-      <c r="G27" s="0" t="s">
+      <c r="G27" s="1" t="s">
         <v>597</v>
       </c>
       <c r="H27" s="1" t="s">
@@ -5417,7 +5440,7 @@
       <c r="F28" s="1" t="s">
         <v>612</v>
       </c>
-      <c r="G28" s="0" t="s">
+      <c r="G28" s="1" t="s">
         <v>613</v>
       </c>
       <c r="H28" s="1" t="s">
@@ -5467,7 +5490,7 @@
       <c r="F29" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="G29" s="0" t="s">
+      <c r="G29" s="1" t="s">
         <v>628</v>
       </c>
       <c r="H29" s="1" t="s">
@@ -5926,7 +5949,7 @@
       <c r="D41" s="1" t="s">
         <v>770</v>
       </c>
-      <c r="E41" s="5" t="s">
+      <c r="E41" s="1" t="s">
         <v>771</v>
       </c>
       <c r="F41" s="4" t="s">
@@ -6290,7 +6313,7 @@
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D55" s="6" t="s">
+      <c r="D55" s="5" t="s">
         <v>882</v>
       </c>
       <c r="H55" s="1" t="s">
@@ -6393,7 +6416,7 @@
       <c r="D60" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="H60" s="7" t="s">
+      <c r="H60" s="6" t="s">
         <v>912</v>
       </c>
       <c r="I60" s="1" t="s">
@@ -6640,7 +6663,7 @@
       <c r="L74" s="1" t="s">
         <v>983</v>
       </c>
-      <c r="Z74" s="7" t="s">
+      <c r="Z74" s="6" t="s">
         <v>984</v>
       </c>
     </row>
@@ -6657,133 +6680,160 @@
       <c r="L75" s="1" t="s">
         <v>988</v>
       </c>
+      <c r="Z75" s="0" t="s">
+        <v>989</v>
+      </c>
     </row>
     <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D76" s="1" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>990</v>
+        <v>991</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="L76" s="1" t="s">
-        <v>992</v>
+        <v>993</v>
+      </c>
+      <c r="Z76" s="0" t="s">
+        <v>994</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D77" s="1" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>994</v>
+        <v>996</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>995</v>
+        <v>997</v>
       </c>
       <c r="L77" s="1" t="s">
-        <v>996</v>
+        <v>998</v>
+      </c>
+      <c r="Z77" s="0" t="s">
+        <v>999</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D78" s="4" t="s">
-        <v>997</v>
+        <v>1000</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>998</v>
+        <v>1001</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>999</v>
+        <v>1002</v>
       </c>
       <c r="L78" s="1" t="s">
-        <v>1000</v>
+        <v>1003</v>
+      </c>
+      <c r="Z78" s="0" t="s">
+        <v>1004</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D79" s="4" t="s">
-        <v>1001</v>
+        <v>1005</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>1002</v>
+        <v>1006</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>1003</v>
+        <v>1007</v>
+      </c>
+      <c r="Z79" s="0" t="s">
+        <v>1008</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D80" s="1" t="s">
-        <v>1004</v>
+        <v>1009</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>1005</v>
+        <v>1010</v>
+      </c>
+      <c r="I80" s="0" t="s">
+        <v>1011</v>
+      </c>
+      <c r="Z80" s="0" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D81" s="1" t="s">
-        <v>1006</v>
+        <v>1013</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>1007</v>
+        <v>1014</v>
+      </c>
+      <c r="I81" s="0" t="s">
+        <v>1015</v>
+      </c>
+      <c r="Z81" s="0" t="s">
+        <v>1016</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D82" s="1" t="s">
-        <v>1008</v>
+        <v>1017</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>1009</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D83" s="1" t="s">
-        <v>1010</v>
-      </c>
-      <c r="H83" s="5" t="s">
-        <v>1011</v>
+        <v>1019</v>
+      </c>
+      <c r="H83" s="1" t="s">
+        <v>1020</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D84" s="1" t="s">
-        <v>1012</v>
+        <v>1021</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>1013</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D85" s="1" t="s">
-        <v>1014</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D86" s="1" t="s">
-        <v>1015</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D87" s="1" t="s">
-        <v>1016</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D88" s="1" t="s">
-        <v>1017</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D89" s="1" t="s">
-        <v>1018</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D90" s="1" t="s">
-        <v>1019</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D91" s="1" t="s">
-        <v>1020</v>
+        <v>1029</v>
       </c>
     </row>
   </sheetData>

</xml_diff>